<commit_message>
Limpando a lista de vencedores
</commit_message>
<xml_diff>
--- a/Sorteio-Toodoo/Sorteio-Toodoo/bin/Debug/net5.0-windows/Winners_List.xlsx
+++ b/Sorteio-Toodoo/Sorteio-Toodoo/bin/Debug/net5.0-windows/Winners_List.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="L:\Joao\CSharp\Toodoo\BlastOff\Projects\Sorteio-Toodoo\Sorteio-Toodoo\bin\Debug\net5.0-windows\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="L:\Joao\CSharp\Toodoo\Sorteio_Aniversario_Toodoo\Sorteio_Aniversario_Toodoo\Sorteio-Toodoo\Sorteio-Toodoo\bin\Debug\net5.0-windows\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,87 +14,16 @@
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
-  <si>
-    <t>Lucas Thalles dos Santos</t>
-  </si>
-  <si>
-    <t>Ygor Guilherme Ribeiro Rosa</t>
-  </si>
-  <si>
-    <t>Guilherme Esquivel dos Santos</t>
-  </si>
-  <si>
-    <t>Matheus Cleber Silva Guerra</t>
-  </si>
-  <si>
-    <t>Roberto Ryan Caldas Ribeiro</t>
-  </si>
-  <si>
-    <t>Paulo Sérgio Aquino Ribeiro</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Diogenes  Aparecido Rezende</t>
-  </si>
-  <si>
-    <t>Tharsis Lamin Lumumba Boa Morte Queiroz</t>
-  </si>
-  <si>
-    <t>Leonardo Everton da Costa</t>
-  </si>
-  <si>
-    <t>Lucas Eduardo Moraes da Silva</t>
-  </si>
-  <si>
-    <t>Marcelo Bruno Verissimo Mendes Moraes Viegas</t>
-  </si>
-  <si>
-    <t>Gabriel Junior de Souza</t>
-  </si>
-  <si>
-    <t>Walber Fellipe de Almeida Rosa</t>
-  </si>
-  <si>
-    <t>Samuel Alves Brandani Tenório</t>
-  </si>
-  <si>
-    <t>Nicole Ribeiro de Paula</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DIEGO ALVES OPENHEIMER </t>
-  </si>
-  <si>
-    <t>Bruno Gabriel Nogueira da Silva</t>
-  </si>
-  <si>
-    <t>Felipe Gabriel da Cunha</t>
-  </si>
-  <si>
-    <t>Patrick Barnabé Moreira Santos</t>
-  </si>
-  <si>
-    <t>João Vitor Alves Lima</t>
-  </si>
-  <si>
-    <t>Ruan Patrick de Souza</t>
-  </si>
-  <si>
-    <t>Gustavo Henrique da Silva Prado</t>
-  </si>
-  <si>
-    <t>Felipe Rafael Tancredi Pascucci</t>
-  </si>
-</sst>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="0"/>
   <fonts count="1">
     <font>
       <sz val="11"/>
@@ -122,7 +51,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -402,132 +331,15 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac xr">
-  <dimension ref="A1:A23"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="0" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="0" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="0" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="0" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="0" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="0" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="0" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="0" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="0" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="0" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="0" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="0" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="0" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" s="0" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" s="0" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" s="0" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" s="0" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" s="0" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" s="0" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" s="0" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" s="0" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" s="0" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" s="0" t="s">
-        <v>22</v>
-      </c>
-    </row>
-  </sheetData>
+  <sheetData/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>